<commit_message>
Working on Optimize project test
</commit_message>
<xml_diff>
--- a/Testing/data/sphere/groom.xlsx
+++ b/Testing/data/sphere/groom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
   <si>
     <t>segmentation_file</t>
   </si>
@@ -191,6 +191,36 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>groomed_file</t>
+  </si>
+  <si>
+    <t>sphere10_DT.nrrd</t>
+  </si>
+  <si>
+    <t>transform_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -0.002400 -0.002400 -0.002400</t>
+  </si>
+  <si>
+    <t>sphere20_DT.nrrd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -0.000599 -0.000599 -0.000599</t>
+  </si>
+  <si>
+    <t>sphere30_DT.nrrd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -0.000265 -0.000265 -0.000265</t>
+  </si>
+  <si>
+    <t>sphere40_DT.nrrd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -0.000149 -0.000149 -0.000149</t>
   </si>
 </sst>
 </file>
@@ -500,35 +530,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>